<commit_message>
Fixed querying issues and added new Gerrit Servers to search through
</commit_message>
<xml_diff>
--- a/backend/controllers/csv/11022-SP12,11160-SP4,ehsxmngmodifiedData.xlsx
+++ b/backend/controllers/csv/11022-SP12,11160-SP4,ehsxmngmodifiedData.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AR5"/>
+  <dimension ref="A1:AR22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -538,13 +538,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>[SP:11022-SP12]</v>
+        <v>[PC]</v>
       </c>
       <c r="B2" t="str">
-        <v>cb7c6bb2aa96937c27ea3cfcf2732b49f729aa1b</v>
+        <v>a611fd99a709bcbbcd26571ca873a9b8c715cbc6</v>
       </c>
       <c r="C2" t="str">
-        <v>https://gerrit.ericsson.se/q/commit:cb7c6bb2aa96937c27ea3cfcf2732b49f729aa1b</v>
+        <v>https://gerrit.ericsson.se/q/commit:a611fd99a709bcbbcd26571ca873a9b8c715cbc6</v>
       </c>
       <c r="D2" t="str">
         <v>gerrit</v>
@@ -565,73 +565,73 @@
         <v>unknown</v>
       </c>
       <c r="J2" t="str">
-        <v>lte/ebb</v>
+        <v>5g/src/rpcppg2</v>
       </c>
       <c r="K2" t="str">
         <v>MSRBS</v>
       </c>
       <c r="L2" t="str">
-        <v>[SP:11022-SP12] Update cellInfoId Interface</v>
+        <v>[PC] Any&lt;T&gt; to std::optional&lt;T&gt; for PucchConfig</v>
       </c>
       <c r="M2" t="str">
-        <v>2023-11-18</v>
+        <v>2023-01-10</v>
       </c>
       <c r="N2" t="str">
-        <v>2023-11-18</v>
+        <v>2023-01-10</v>
       </c>
       <c r="O2" t="str">
-        <v>source</v>
+        <v>source test</v>
       </c>
       <c r="P2">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="R2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S2">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="T2">
+        <v>8</v>
+      </c>
+      <c r="U2">
+        <v>23</v>
+      </c>
+      <c r="V2">
+        <v>24</v>
+      </c>
+      <c r="W2">
+        <v>-1</v>
+      </c>
+      <c r="X2">
+        <v>47</v>
+      </c>
+      <c r="Y2">
+        <v>8</v>
+      </c>
+      <c r="Z2">
+        <v>69</v>
+      </c>
+      <c r="AA2">
+        <v>68</v>
+      </c>
+      <c r="AB2">
         <v>1</v>
       </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>4</v>
-      </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
-      <c r="AB2">
-        <v>4</v>
-      </c>
       <c r="AC2">
-        <v>4</v>
+        <v>137</v>
       </c>
       <c r="AD2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="AE2">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="AF2">
-        <v>2.07</v>
+        <v>2.42</v>
       </c>
       <c r="AG2">
         <v>0</v>
@@ -642,13 +642,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>[SP:11022-SP12]</v>
+        <v>[PC]</v>
       </c>
       <c r="B3" t="str">
-        <v>236fd51082f64ea82e70fd52f04841af3463f820</v>
+        <v>e01c4bfff82d2b254a864f32845e65a8b1529cf0</v>
       </c>
       <c r="C3" t="str">
-        <v>https://gerrit.ericsson.se/q/commit:236fd51082f64ea82e70fd52f04841af3463f820</v>
+        <v>https://gerrit.ericsson.se/q/commit:e01c4bfff82d2b254a864f32845e65a8b1529cf0</v>
       </c>
       <c r="D3" t="str">
         <v>gerrit</v>
@@ -669,93 +669,93 @@
         <v>unknown</v>
       </c>
       <c r="J3" t="str">
-        <v>lte/ebb</v>
+        <v>5g/src/rpcppg2</v>
       </c>
       <c r="K3" t="str">
         <v>MSRBS</v>
       </c>
       <c r="L3" t="str">
-        <v>[SP:11022-SP12] AggresiveUss SCs</v>
+        <v>[PC] Any&lt;T&gt; to sdt::optional&lt;T&gt; in rrc</v>
       </c>
       <c r="M3" t="str">
-        <v>2023-12-16</v>
+        <v>2023-01-23</v>
       </c>
       <c r="N3" t="str">
-        <v>2023-12-16</v>
+        <v>2023-01-24</v>
       </c>
       <c r="O3" t="str">
         <v>source test</v>
       </c>
       <c r="P3">
-        <v>184</v>
+        <v>97</v>
       </c>
       <c r="Q3">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="R3">
-        <v>181</v>
+        <v>-6</v>
       </c>
       <c r="S3">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="T3">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="U3">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="W3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="X3">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="Y3">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="Z3">
-        <v>192</v>
+        <v>131</v>
       </c>
       <c r="AA3">
-        <v>3</v>
+        <v>136</v>
       </c>
       <c r="AB3">
-        <v>189</v>
+        <v>-5</v>
       </c>
       <c r="AC3">
-        <v>195</v>
+        <v>267</v>
       </c>
       <c r="AD3">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="AE3">
-        <v>72.73</v>
+        <v>0.88</v>
       </c>
       <c r="AF3">
-        <v>98.96</v>
+        <v>7.8</v>
       </c>
       <c r="AG3">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="AH3">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="AI3">
-        <v>0.04</v>
+        <v>0.07</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>[SP:11022-SP12]</v>
+        <v>[PC]</v>
       </c>
       <c r="B4" t="str">
-        <v>3f751ade39a5776e1de9e55a65b132c586343e0a</v>
+        <v>cf74d456e04e50934dad680b361e9fba0e2d9d93</v>
       </c>
       <c r="C4" t="str">
-        <v>https://gerrit.ericsson.se/q/commit:3f751ade39a5776e1de9e55a65b132c586343e0a</v>
+        <v>https://gerrit.ericsson.se/q/commit:cf74d456e04e50934dad680b361e9fba0e2d9d93</v>
       </c>
       <c r="D4" t="str">
         <v>gerrit</v>
@@ -776,116 +776,1935 @@
         <v>unknown</v>
       </c>
       <c r="J4" t="str">
-        <v>lte/ebb</v>
+        <v>5g/src/rpcppg2</v>
       </c>
       <c r="K4" t="str">
         <v>MSRBS</v>
       </c>
       <c r="L4" t="str">
-        <v>[SP:11022-SP12] AggresiveUss SCs Fix</v>
+        <v>[PC] Replace Any with std::optional</v>
       </c>
       <c r="M4" t="str">
-        <v>2023-12-20</v>
+        <v>2023-03-16</v>
       </c>
       <c r="N4" t="str">
-        <v>2023-12-20</v>
+        <v>2023-03-16</v>
       </c>
       <c r="O4" t="str">
         <v>source test</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="Q4">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>-12</v>
       </c>
       <c r="S4">
-        <v>2</v>
+        <v>126</v>
       </c>
       <c r="T4">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="V4">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="W4">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="X4">
-        <v>3</v>
+        <v>296</v>
       </c>
       <c r="Y4">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="Z4">
-        <v>1</v>
+        <v>204</v>
       </c>
       <c r="AA4">
-        <v>4</v>
+        <v>218</v>
       </c>
       <c r="AB4">
-        <v>-3</v>
+        <v>-14</v>
       </c>
       <c r="AC4">
-        <v>5</v>
+        <v>422</v>
       </c>
       <c r="AD4">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="AE4">
-        <v>100</v>
+        <v>3.18</v>
       </c>
       <c r="AF4">
-        <v>100</v>
+        <v>11.18</v>
       </c>
       <c r="AG4">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="AH4">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="AI4">
-        <v>0.25</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="5">
-      <c r="AJ5">
-        <v>32</v>
-      </c>
-      <c r="AK5" t="str">
-        <v>2023-11-18</v>
-      </c>
-      <c r="AL5" t="str">
-        <v>2023-12-20</v>
-      </c>
-      <c r="AM5">
-        <v>193</v>
-      </c>
-      <c r="AN5">
-        <v>11</v>
-      </c>
-      <c r="AO5">
+      <c r="A5" t="str">
+        <v>[SP:10181-2]</v>
+      </c>
+      <c r="B5" t="str">
+        <v>1e7ea84e21b4910b1d1bbe3c173f19af475fe0b6</v>
+      </c>
+      <c r="C5" t="str">
+        <v>https://gerrit.ericsson.se/q/commit:1e7ea84e21b4910b1d1bbe3c173f19af475fe0b6</v>
+      </c>
+      <c r="D5" t="str">
+        <v>gerrit</v>
+      </c>
+      <c r="E5" t="str">
+        <v>ehsxmng</v>
+      </c>
+      <c r="F5" t="str">
+        <v>Ming-Chen Hsu</v>
+      </c>
+      <c r="G5" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="H5" t="str">
+        <v>Unknown</v>
+      </c>
+      <c r="I5" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="J5" t="str">
+        <v>5g/src/rpcppg2</v>
+      </c>
+      <c r="K5" t="str">
+        <v>MSRBS</v>
+      </c>
+      <c r="L5" t="str">
+        <v>[SP:10181-2] Removal of rpcControl SC</v>
+      </c>
+      <c r="M5" t="str">
+        <v>2023-04-20</v>
+      </c>
+      <c r="N5" t="str">
+        <v>2023-04-20</v>
+      </c>
+      <c r="O5" t="str">
+        <v>source test</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>14</v>
+      </c>
+      <c r="R5">
+        <v>-14</v>
+      </c>
+      <c r="S5">
+        <v>14</v>
+      </c>
+      <c r="T5">
+        <v>3</v>
+      </c>
+      <c r="U5">
+        <v>24</v>
+      </c>
+      <c r="V5">
+        <v>64</v>
+      </c>
+      <c r="W5">
+        <v>-40</v>
+      </c>
+      <c r="X5">
+        <v>88</v>
+      </c>
+      <c r="Y5">
+        <v>5</v>
+      </c>
+      <c r="Z5">
+        <v>24</v>
+      </c>
+      <c r="AA5">
+        <v>78</v>
+      </c>
+      <c r="AB5">
+        <v>-54</v>
+      </c>
+      <c r="AC5">
+        <v>102</v>
+      </c>
+      <c r="AD5">
+        <v>8</v>
+      </c>
+      <c r="AE5">
+        <v>3.86</v>
+      </c>
+      <c r="AF5">
+        <v>11.56</v>
+      </c>
+      <c r="AG5">
+        <v>100</v>
+      </c>
+      <c r="AH5">
+        <v>35</v>
+      </c>
+      <c r="AI5">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>[SP:10181-2]</v>
+      </c>
+      <c r="B6" t="str">
+        <v>0f919abe5307e91e1c4bba0cd7c5bb41a8c4c788</v>
+      </c>
+      <c r="C6" t="str">
+        <v>https://gerrit.ericsson.se/q/commit:0f919abe5307e91e1c4bba0cd7c5bb41a8c4c788</v>
+      </c>
+      <c r="D6" t="str">
+        <v>gerrit</v>
+      </c>
+      <c r="E6" t="str">
+        <v>ehsxmng</v>
+      </c>
+      <c r="F6" t="str">
+        <v>Ming-Chen Hsu</v>
+      </c>
+      <c r="G6" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="H6" t="str">
+        <v>Unknown</v>
+      </c>
+      <c r="I6" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="J6" t="str">
+        <v>5g/src/rpcppg2</v>
+      </c>
+      <c r="K6" t="str">
+        <v>MSRBS</v>
+      </c>
+      <c r="L6" t="str">
+        <v>[SP:10181-2] Remove sc for T+T+F+F CA combo</v>
+      </c>
+      <c r="M6" t="str">
+        <v>2023-05-02</v>
+      </c>
+      <c r="N6" t="str">
+        <v>2023-05-02</v>
+      </c>
+      <c r="O6" t="str">
+        <v>source</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>102</v>
+      </c>
+      <c r="R6">
+        <v>-101</v>
+      </c>
+      <c r="S6">
+        <v>103</v>
+      </c>
+      <c r="T6">
+        <v>4</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>102</v>
+      </c>
+      <c r="AB6">
+        <v>-101</v>
+      </c>
+      <c r="AC6">
+        <v>103</v>
+      </c>
+      <c r="AD6">
+        <v>4</v>
+      </c>
+      <c r="AE6">
+        <v>3.86</v>
+      </c>
+      <c r="AF6">
+        <v>14.33</v>
+      </c>
+      <c r="AG6">
+        <v>112</v>
+      </c>
+      <c r="AH6">
+        <v>12</v>
+      </c>
+      <c r="AI6">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>[SP:11022-SP6]</v>
+      </c>
+      <c r="B7" t="str">
+        <v>d87e06a41090d2ddac3fd3e0b438f4d00c034ef2</v>
+      </c>
+      <c r="C7" t="str">
+        <v>https://gerrit.ericsson.se/q/commit:d87e06a41090d2ddac3fd3e0b438f4d00c034ef2</v>
+      </c>
+      <c r="D7" t="str">
+        <v>gerrit</v>
+      </c>
+      <c r="E7" t="str">
+        <v>ehsxmng</v>
+      </c>
+      <c r="F7" t="str">
+        <v>Ming-Chen Hsu</v>
+      </c>
+      <c r="G7" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="H7" t="str">
+        <v>Unknown</v>
+      </c>
+      <c r="I7" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="J7" t="str">
+        <v>5g/src/ucl</v>
+      </c>
+      <c r="K7" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="L7" t="str">
+        <v>[SP:11022-SP6] Add DMRS Type support</v>
+      </c>
+      <c r="M7" t="str">
+        <v>2023-07-05</v>
+      </c>
+      <c r="N7" t="str">
+        <v>2023-07-05</v>
+      </c>
+      <c r="O7" t="str">
+        <v>source test</v>
+      </c>
+      <c r="P7">
+        <v>144</v>
+      </c>
+      <c r="Q7">
+        <v>6</v>
+      </c>
+      <c r="R7">
+        <v>138</v>
+      </c>
+      <c r="S7">
+        <v>150</v>
+      </c>
+      <c r="T7">
+        <v>5</v>
+      </c>
+      <c r="U7">
+        <v>167</v>
+      </c>
+      <c r="V7">
+        <v>29</v>
+      </c>
+      <c r="W7">
+        <v>138</v>
+      </c>
+      <c r="X7">
+        <v>196</v>
+      </c>
+      <c r="Y7">
+        <v>19</v>
+      </c>
+      <c r="Z7">
+        <v>311</v>
+      </c>
+      <c r="AA7">
+        <v>35</v>
+      </c>
+      <c r="AB7">
+        <v>276</v>
+      </c>
+      <c r="AC7">
+        <v>346</v>
+      </c>
+      <c r="AD7">
+        <v>24</v>
+      </c>
+      <c r="AE7">
+        <v>5.38</v>
+      </c>
+      <c r="AF7">
+        <v>18.36</v>
+      </c>
+      <c r="AG7">
+        <v>176</v>
+      </c>
+      <c r="AH7">
+        <v>64</v>
+      </c>
+      <c r="AI7">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>[PC]</v>
+      </c>
+      <c r="B8" t="str">
+        <v>9af025d3420cafc02b2da822cece7b72f5f17f11</v>
+      </c>
+      <c r="C8" t="str">
+        <v>https://gerrit.ericsson.se/q/commit:9af025d3420cafc02b2da822cece7b72f5f17f11</v>
+      </c>
+      <c r="D8" t="str">
+        <v>gerrit</v>
+      </c>
+      <c r="E8" t="str">
+        <v>ehsxmng</v>
+      </c>
+      <c r="F8" t="str">
+        <v>Ming-Chen Hsu</v>
+      </c>
+      <c r="G8" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="H8" t="str">
+        <v>Unknown</v>
+      </c>
+      <c r="I8" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="J8" t="str">
+        <v>5g/src/rpcppg2</v>
+      </c>
+      <c r="K8" t="str">
+        <v>MSRBS</v>
+      </c>
+      <c r="L8" t="str">
+        <v>[PC] Replace Any with optional</v>
+      </c>
+      <c r="M8" t="str">
+        <v>2023-07-26</v>
+      </c>
+      <c r="N8" t="str">
+        <v>2023-07-26</v>
+      </c>
+      <c r="O8" t="str">
+        <v>source test</v>
+      </c>
+      <c r="P8">
+        <v>259</v>
+      </c>
+      <c r="Q8">
+        <v>269</v>
+      </c>
+      <c r="R8">
+        <v>-10</v>
+      </c>
+      <c r="S8">
+        <v>528</v>
+      </c>
+      <c r="T8">
+        <v>59</v>
+      </c>
+      <c r="U8">
+        <v>315</v>
+      </c>
+      <c r="V8">
+        <v>286</v>
+      </c>
+      <c r="W8">
+        <v>29</v>
+      </c>
+      <c r="X8">
+        <v>601</v>
+      </c>
+      <c r="Y8">
+        <v>63</v>
+      </c>
+      <c r="Z8">
+        <v>574</v>
+      </c>
+      <c r="AA8">
+        <v>555</v>
+      </c>
+      <c r="AB8">
+        <v>19</v>
+      </c>
+      <c r="AC8">
+        <v>1129</v>
+      </c>
+      <c r="AD8">
+        <v>122</v>
+      </c>
+      <c r="AE8">
+        <v>10.03</v>
+      </c>
+      <c r="AF8">
+        <v>32.55</v>
+      </c>
+      <c r="AG8">
+        <v>197</v>
+      </c>
+      <c r="AH8">
+        <v>21</v>
+      </c>
+      <c r="AI8">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>[PC]</v>
+      </c>
+      <c r="B9" t="str">
+        <v>2407ae9e66644c114ea2cc19bb0af37b44cb2e59</v>
+      </c>
+      <c r="C9" t="str">
+        <v>https://gerrit.ericsson.se/q/commit:2407ae9e66644c114ea2cc19bb0af37b44cb2e59</v>
+      </c>
+      <c r="D9" t="str">
+        <v>gerrit</v>
+      </c>
+      <c r="E9" t="str">
+        <v>ehsxmng</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Ming-Chen Hsu</v>
+      </c>
+      <c r="G9" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="H9" t="str">
+        <v>Unknown</v>
+      </c>
+      <c r="I9" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="J9" t="str">
+        <v>5g/src/rpcppg2</v>
+      </c>
+      <c r="K9" t="str">
+        <v>MSRBS</v>
+      </c>
+      <c r="L9" t="str">
+        <v>[PC] Replace Any with optional</v>
+      </c>
+      <c r="M9" t="str">
+        <v>2023-08-02</v>
+      </c>
+      <c r="N9" t="str">
+        <v>2023-08-02</v>
+      </c>
+      <c r="O9" t="str">
+        <v>source test</v>
+      </c>
+      <c r="P9">
+        <v>99</v>
+      </c>
+      <c r="Q9">
+        <v>113</v>
+      </c>
+      <c r="R9">
+        <v>-14</v>
+      </c>
+      <c r="S9">
+        <v>212</v>
+      </c>
+      <c r="T9">
+        <v>35</v>
+      </c>
+      <c r="U9">
+        <v>189</v>
+      </c>
+      <c r="V9">
+        <v>161</v>
+      </c>
+      <c r="W9">
+        <v>28</v>
+      </c>
+      <c r="X9">
+        <v>350</v>
+      </c>
+      <c r="Y9">
+        <v>27</v>
+      </c>
+      <c r="Z9">
+        <v>288</v>
+      </c>
+      <c r="AA9">
+        <v>274</v>
+      </c>
+      <c r="AB9">
+        <v>14</v>
+      </c>
+      <c r="AC9">
+        <v>562</v>
+      </c>
+      <c r="AD9">
+        <v>62</v>
+      </c>
+      <c r="AE9">
+        <v>12.74</v>
+      </c>
+      <c r="AF9">
+        <v>38.25</v>
+      </c>
+      <c r="AG9">
         <v>204</v>
       </c>
-      <c r="AP5">
+      <c r="AH9">
+        <v>7</v>
+      </c>
+      <c r="AI9">
+        <v>0.14</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>[PC]</v>
+      </c>
+      <c r="B10" t="str">
+        <v>71debfe1cb672a2d39ce7cc71fc0728d2838937e</v>
+      </c>
+      <c r="C10" t="str">
+        <v>https://gerrit.ericsson.se/q/commit:71debfe1cb672a2d39ce7cc71fc0728d2838937e</v>
+      </c>
+      <c r="D10" t="str">
+        <v>gerrit</v>
+      </c>
+      <c r="E10" t="str">
+        <v>ehsxmng</v>
+      </c>
+      <c r="F10" t="str">
+        <v>Ming-Chen Hsu</v>
+      </c>
+      <c r="G10" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="H10" t="str">
+        <v>Unknown</v>
+      </c>
+      <c r="I10" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="J10" t="str">
+        <v>5g/src/rpcppg2</v>
+      </c>
+      <c r="K10" t="str">
+        <v>MSRBS</v>
+      </c>
+      <c r="L10" t="str">
+        <v>[PC] Replace Any with optional</v>
+      </c>
+      <c r="M10" t="str">
+        <v>2023-08-14</v>
+      </c>
+      <c r="N10" t="str">
+        <v>2023-08-14</v>
+      </c>
+      <c r="O10" t="str">
+        <v>source test</v>
+      </c>
+      <c r="P10">
+        <v>162</v>
+      </c>
+      <c r="Q10">
+        <v>175</v>
+      </c>
+      <c r="R10">
+        <v>-13</v>
+      </c>
+      <c r="S10">
+        <v>337</v>
+      </c>
+      <c r="T10">
+        <v>24</v>
+      </c>
+      <c r="U10">
+        <v>2079</v>
+      </c>
+      <c r="V10">
+        <v>2029</v>
+      </c>
+      <c r="W10">
+        <v>50</v>
+      </c>
+      <c r="X10">
+        <v>4108</v>
+      </c>
+      <c r="Y10">
+        <v>38</v>
+      </c>
+      <c r="Z10">
+        <v>2241</v>
+      </c>
+      <c r="AA10">
+        <v>2204</v>
+      </c>
+      <c r="AB10">
+        <v>37</v>
+      </c>
+      <c r="AC10">
+        <v>4445</v>
+      </c>
+      <c r="AD10">
+        <v>62</v>
+      </c>
+      <c r="AE10">
+        <v>44.57</v>
+      </c>
+      <c r="AF10">
+        <v>47.31</v>
+      </c>
+      <c r="AG10">
+        <v>216</v>
+      </c>
+      <c r="AH10">
+        <v>12</v>
+      </c>
+      <c r="AI10">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>[PC]</v>
+      </c>
+      <c r="B11" t="str">
+        <v>4e01b5ad0e30d414c4008c9e552ec96238cc9619</v>
+      </c>
+      <c r="C11" t="str">
+        <v>https://gerrit.ericsson.se/q/commit:4e01b5ad0e30d414c4008c9e552ec96238cc9619</v>
+      </c>
+      <c r="D11" t="str">
+        <v>gerrit</v>
+      </c>
+      <c r="E11" t="str">
+        <v>ehsxmng</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Ming-Chen Hsu</v>
+      </c>
+      <c r="G11" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="H11" t="str">
+        <v>Unknown</v>
+      </c>
+      <c r="I11" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="J11" t="str">
+        <v>5g/src/rpcppg2</v>
+      </c>
+      <c r="K11" t="str">
+        <v>MSRBS</v>
+      </c>
+      <c r="L11" t="str">
+        <v>[PC] Replace Any with optional</v>
+      </c>
+      <c r="M11" t="str">
+        <v>2023-08-16</v>
+      </c>
+      <c r="N11" t="str">
+        <v>2023-08-16</v>
+      </c>
+      <c r="O11" t="str">
+        <v>source test</v>
+      </c>
+      <c r="P11">
+        <v>108</v>
+      </c>
+      <c r="Q11">
+        <v>111</v>
+      </c>
+      <c r="R11">
+        <v>-3</v>
+      </c>
+      <c r="S11">
+        <v>219</v>
+      </c>
+      <c r="T11">
+        <v>12</v>
+      </c>
+      <c r="U11">
+        <v>1687</v>
+      </c>
+      <c r="V11">
+        <v>1675</v>
+      </c>
+      <c r="W11">
+        <v>12</v>
+      </c>
+      <c r="X11">
+        <v>3362</v>
+      </c>
+      <c r="Y11">
+        <v>24</v>
+      </c>
+      <c r="Z11">
+        <v>1795</v>
+      </c>
+      <c r="AA11">
+        <v>1786</v>
+      </c>
+      <c r="AB11">
+        <v>9</v>
+      </c>
+      <c r="AC11">
+        <v>3581</v>
+      </c>
+      <c r="AD11">
+        <v>36</v>
+      </c>
+      <c r="AE11">
+        <v>70.62</v>
+      </c>
+      <c r="AF11">
+        <v>53.2</v>
+      </c>
+      <c r="AG11">
+        <v>218</v>
+      </c>
+      <c r="AH11">
+        <v>2</v>
+      </c>
+      <c r="AI11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>[PC]</v>
+      </c>
+      <c r="B12" t="str">
+        <v>723a1ed4e159ea4edeb2ad3d4d1ffd9645c18328</v>
+      </c>
+      <c r="C12" t="str">
+        <v>https://gerrit.ericsson.se/q/commit:723a1ed4e159ea4edeb2ad3d4d1ffd9645c18328</v>
+      </c>
+      <c r="D12" t="str">
+        <v>gerrit</v>
+      </c>
+      <c r="E12" t="str">
+        <v>ehsxmng</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Ming-Chen Hsu</v>
+      </c>
+      <c r="G12" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="H12" t="str">
+        <v>Unknown</v>
+      </c>
+      <c r="I12" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="J12" t="str">
+        <v>5g/src/rpcppg2</v>
+      </c>
+      <c r="K12" t="str">
+        <v>MSRBS</v>
+      </c>
+      <c r="L12" t="str">
+        <v>[PC] Replace Any with optional</v>
+      </c>
+      <c r="M12" t="str">
+        <v>2023-08-22</v>
+      </c>
+      <c r="N12" t="str">
+        <v>2023-08-22</v>
+      </c>
+      <c r="O12" t="str">
+        <v>source test</v>
+      </c>
+      <c r="P12">
+        <v>175</v>
+      </c>
+      <c r="Q12">
+        <v>178</v>
+      </c>
+      <c r="R12">
+        <v>-3</v>
+      </c>
+      <c r="S12">
+        <v>353</v>
+      </c>
+      <c r="T12">
+        <v>24</v>
+      </c>
+      <c r="U12">
+        <v>348</v>
+      </c>
+      <c r="V12">
+        <v>411</v>
+      </c>
+      <c r="W12">
+        <v>-63</v>
+      </c>
+      <c r="X12">
+        <v>759</v>
+      </c>
+      <c r="Y12">
+        <v>30</v>
+      </c>
+      <c r="Z12">
+        <v>523</v>
+      </c>
+      <c r="AA12">
+        <v>589</v>
+      </c>
+      <c r="AB12">
+        <v>-66</v>
+      </c>
+      <c r="AC12">
+        <v>1112</v>
+      </c>
+      <c r="AD12">
+        <v>54</v>
+      </c>
+      <c r="AE12">
+        <v>76.5</v>
+      </c>
+      <c r="AF12">
+        <v>62.69</v>
+      </c>
+      <c r="AG12">
+        <v>224</v>
+      </c>
+      <c r="AH12">
+        <v>6</v>
+      </c>
+      <c r="AI12">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>[PC]</v>
+      </c>
+      <c r="B13" t="str">
+        <v>b5ce5fcf7153a09a979e84554ca4bc6b2c790d72</v>
+      </c>
+      <c r="C13" t="str">
+        <v>https://gerrit.ericsson.se/q/commit:b5ce5fcf7153a09a979e84554ca4bc6b2c790d72</v>
+      </c>
+      <c r="D13" t="str">
+        <v>gerrit</v>
+      </c>
+      <c r="E13" t="str">
+        <v>ehsxmng</v>
+      </c>
+      <c r="F13" t="str">
+        <v>Ming-Chen Hsu</v>
+      </c>
+      <c r="G13" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="H13" t="str">
+        <v>Unknown</v>
+      </c>
+      <c r="I13" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="J13" t="str">
+        <v>5g/src/rpcppg2</v>
+      </c>
+      <c r="K13" t="str">
+        <v>MSRBS</v>
+      </c>
+      <c r="L13" t="str">
+        <v>[PC] Replace Any with optional</v>
+      </c>
+      <c r="M13" t="str">
+        <v>2023-09-07</v>
+      </c>
+      <c r="N13" t="str">
+        <v>2023-09-07</v>
+      </c>
+      <c r="O13" t="str">
+        <v>source test</v>
+      </c>
+      <c r="P13">
+        <v>216</v>
+      </c>
+      <c r="Q13">
+        <v>216</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>432</v>
+      </c>
+      <c r="T13">
+        <v>18</v>
+      </c>
+      <c r="U13">
+        <v>708</v>
+      </c>
+      <c r="V13">
+        <v>704</v>
+      </c>
+      <c r="W13">
+        <v>4</v>
+      </c>
+      <c r="X13">
+        <v>1412</v>
+      </c>
+      <c r="Y13">
+        <v>24</v>
+      </c>
+      <c r="Z13">
+        <v>924</v>
+      </c>
+      <c r="AA13">
+        <v>920</v>
+      </c>
+      <c r="AB13">
+        <v>4</v>
+      </c>
+      <c r="AC13">
+        <v>1844</v>
+      </c>
+      <c r="AD13">
+        <v>42</v>
+      </c>
+      <c r="AE13">
+        <v>87.43</v>
+      </c>
+      <c r="AF13">
+        <v>74.3</v>
+      </c>
+      <c r="AG13">
+        <v>240</v>
+      </c>
+      <c r="AH13">
+        <v>16</v>
+      </c>
+      <c r="AI13">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>[PC]</v>
+      </c>
+      <c r="B14" t="str">
+        <v>deb4bca6e57c095e2f3886b61be6b901c5bba929</v>
+      </c>
+      <c r="C14" t="str">
+        <v>https://gerrit.ericsson.se/q/commit:deb4bca6e57c095e2f3886b61be6b901c5bba929</v>
+      </c>
+      <c r="D14" t="str">
+        <v>gerrit</v>
+      </c>
+      <c r="E14" t="str">
+        <v>ehsxmng</v>
+      </c>
+      <c r="F14" t="str">
+        <v>Ming-Chen Hsu</v>
+      </c>
+      <c r="G14" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="H14" t="str">
+        <v>Unknown</v>
+      </c>
+      <c r="I14" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="J14" t="str">
+        <v>5g/src/rpcppg2</v>
+      </c>
+      <c r="K14" t="str">
+        <v>MSRBS</v>
+      </c>
+      <c r="L14" t="str">
+        <v>[PC] Replace Any with optional</v>
+      </c>
+      <c r="M14" t="str">
+        <v>2023-09-14</v>
+      </c>
+      <c r="N14" t="str">
+        <v>2023-09-14</v>
+      </c>
+      <c r="O14" t="str">
+        <v>source test</v>
+      </c>
+      <c r="P14">
+        <v>148</v>
+      </c>
+      <c r="Q14">
+        <v>146</v>
+      </c>
+      <c r="R14">
+        <v>2</v>
+      </c>
+      <c r="S14">
+        <v>294</v>
+      </c>
+      <c r="T14">
+        <v>40</v>
+      </c>
+      <c r="U14">
+        <v>239</v>
+      </c>
+      <c r="V14">
+        <v>234</v>
+      </c>
+      <c r="W14">
+        <v>5</v>
+      </c>
+      <c r="X14">
+        <v>473</v>
+      </c>
+      <c r="Y14">
+        <v>40</v>
+      </c>
+      <c r="Z14">
+        <v>387</v>
+      </c>
+      <c r="AA14">
+        <v>380</v>
+      </c>
+      <c r="AB14">
+        <v>7</v>
+      </c>
+      <c r="AC14">
+        <v>767</v>
+      </c>
+      <c r="AD14">
+        <v>80</v>
+      </c>
+      <c r="AE14">
+        <v>91.1</v>
+      </c>
+      <c r="AF14">
+        <v>82.2</v>
+      </c>
+      <c r="AG14">
+        <v>247</v>
+      </c>
+      <c r="AH14">
+        <v>7</v>
+      </c>
+      <c r="AI14">
+        <v>0.14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>[TCUEPC-437]</v>
+      </c>
+      <c r="B15" t="str">
+        <v>931e9c2c5e68a63517819276d7eb96bd5f641120</v>
+      </c>
+      <c r="C15" t="str">
+        <v>https://gerrit.ericsson.se/q/commit:931e9c2c5e68a63517819276d7eb96bd5f641120</v>
+      </c>
+      <c r="D15" t="str">
+        <v>gerrit</v>
+      </c>
+      <c r="E15" t="str">
+        <v>ehsxmng</v>
+      </c>
+      <c r="F15" t="str">
+        <v>Ming-Chen Hsu</v>
+      </c>
+      <c r="G15" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="H15" t="str">
+        <v>Unknown</v>
+      </c>
+      <c r="I15" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="J15" t="str">
+        <v>5g/src/rpcppg2</v>
+      </c>
+      <c r="K15" t="str">
+        <v>MSRBS</v>
+      </c>
+      <c r="L15" t="str">
+        <v>[TCUEPC-437] coverage for rsrp_util</v>
+      </c>
+      <c r="M15" t="str">
+        <v>2023-11-27</v>
+      </c>
+      <c r="N15" t="str">
+        <v>2023-11-27</v>
+      </c>
+      <c r="O15" t="str">
+        <v>test</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>5</v>
+      </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
+      <c r="W15">
+        <v>4</v>
+      </c>
+      <c r="X15">
+        <v>6</v>
+      </c>
+      <c r="Y15">
+        <v>1</v>
+      </c>
+      <c r="Z15">
+        <v>5</v>
+      </c>
+      <c r="AA15">
+        <v>1</v>
+      </c>
+      <c r="AB15">
+        <v>4</v>
+      </c>
+      <c r="AC15">
+        <v>6</v>
+      </c>
+      <c r="AD15">
+        <v>1</v>
+      </c>
+      <c r="AE15">
+        <v>91.15</v>
+      </c>
+      <c r="AF15">
+        <v>82.2</v>
+      </c>
+      <c r="AG15">
+        <v>321</v>
+      </c>
+      <c r="AH15">
+        <v>74</v>
+      </c>
+      <c r="AI15">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>[TCUEPC-437]</v>
+      </c>
+      <c r="B16" t="str">
+        <v>9ce191a79a775c8852fcfe48cca23d80e818fe19</v>
+      </c>
+      <c r="C16" t="str">
+        <v>https://gerrit.ericsson.se/q/commit:9ce191a79a775c8852fcfe48cca23d80e818fe19</v>
+      </c>
+      <c r="D16" t="str">
+        <v>gerrit</v>
+      </c>
+      <c r="E16" t="str">
+        <v>ehsxmng</v>
+      </c>
+      <c r="F16" t="str">
+        <v>Ming-Chen Hsu</v>
+      </c>
+      <c r="G16" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="H16" t="str">
+        <v>Unknown</v>
+      </c>
+      <c r="I16" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="J16" t="str">
+        <v>5g/src/rpcppg2</v>
+      </c>
+      <c r="K16" t="str">
+        <v>MSRBS</v>
+      </c>
+      <c r="L16" t="str">
+        <v>[TCUEPC-437] Coverage for additional_service_info</v>
+      </c>
+      <c r="M16" t="str">
+        <v>2023-12-05</v>
+      </c>
+      <c r="N16" t="str">
+        <v>2023-12-05</v>
+      </c>
+      <c r="O16" t="str">
+        <v>test</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>48</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>48</v>
+      </c>
+      <c r="X16">
+        <v>48</v>
+      </c>
+      <c r="Y16">
+        <v>1</v>
+      </c>
+      <c r="Z16">
+        <v>48</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>48</v>
+      </c>
+      <c r="AC16">
+        <v>48</v>
+      </c>
+      <c r="AD16">
+        <v>1</v>
+      </c>
+      <c r="AE16">
+        <v>91.52</v>
+      </c>
+      <c r="AF16">
+        <v>82.2</v>
+      </c>
+      <c r="AG16">
+        <v>329</v>
+      </c>
+      <c r="AH16">
         <v>8</v>
       </c>
-      <c r="AQ5">
-        <v>48.25</v>
-      </c>
-      <c r="AR5">
-        <v>2.75</v>
+      <c r="AI16">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>[TCUEPC-437]</v>
+      </c>
+      <c r="B17" t="str">
+        <v>35354cef8db0d7966ec27f40f6f8908fbd609638</v>
+      </c>
+      <c r="C17" t="str">
+        <v>https://gerrit.ericsson.se/q/commit:35354cef8db0d7966ec27f40f6f8908fbd609638</v>
+      </c>
+      <c r="D17" t="str">
+        <v>gerrit</v>
+      </c>
+      <c r="E17" t="str">
+        <v>ehsxmng</v>
+      </c>
+      <c r="F17" t="str">
+        <v>Ming-Chen Hsu</v>
+      </c>
+      <c r="G17" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="H17" t="str">
+        <v>Unknown</v>
+      </c>
+      <c r="I17" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="J17" t="str">
+        <v>5g/src/rpcppg2</v>
+      </c>
+      <c r="K17" t="str">
+        <v>MSRBS</v>
+      </c>
+      <c r="L17" t="str">
+        <v>[TCUEPC-437] Coverage for scells_util</v>
+      </c>
+      <c r="M17" t="str">
+        <v>2024-01-08</v>
+      </c>
+      <c r="N17" t="str">
+        <v>2024-01-08</v>
+      </c>
+      <c r="O17" t="str">
+        <v>test</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>173</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>173</v>
+      </c>
+      <c r="X17">
+        <v>173</v>
+      </c>
+      <c r="Y17">
+        <v>1</v>
+      </c>
+      <c r="Z17">
+        <v>173</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17">
+        <v>173</v>
+      </c>
+      <c r="AC17">
+        <v>173</v>
+      </c>
+      <c r="AD17">
+        <v>1</v>
+      </c>
+      <c r="AE17">
+        <v>92.86</v>
+      </c>
+      <c r="AF17">
+        <v>82.2</v>
+      </c>
+      <c r="AG17">
+        <v>363</v>
+      </c>
+      <c r="AH17">
+        <v>34</v>
+      </c>
+      <c r="AI17">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>[SP:11023-SP2]</v>
+      </c>
+      <c r="B18" t="str">
+        <v>24916b53d08418c514f3978ea784a1ac0a9ffda7</v>
+      </c>
+      <c r="C18" t="str">
+        <v>https://gerrit.ericsson.se/q/commit:24916b53d08418c514f3978ea784a1ac0a9ffda7</v>
+      </c>
+      <c r="D18" t="str">
+        <v>gerrit</v>
+      </c>
+      <c r="E18" t="str">
+        <v>ehsxmng</v>
+      </c>
+      <c r="F18" t="str">
+        <v>Ming-Chen Hsu</v>
+      </c>
+      <c r="G18" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="H18" t="str">
+        <v>Unknown</v>
+      </c>
+      <c r="I18" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="J18" t="str">
+        <v>lte/ebb</v>
+      </c>
+      <c r="K18" t="str">
+        <v>MSRBS</v>
+      </c>
+      <c r="L18" t="str">
+        <v>[SP:11023-SP2] SC for delayTx</v>
+      </c>
+      <c r="M18" t="str">
+        <v>2024-02-06</v>
+      </c>
+      <c r="N18" t="str">
+        <v>2024-02-06</v>
+      </c>
+      <c r="O18" t="str">
+        <v>source test</v>
+      </c>
+      <c r="P18">
+        <v>328</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>328</v>
+      </c>
+      <c r="S18">
+        <v>328</v>
+      </c>
+      <c r="T18">
+        <v>5</v>
+      </c>
+      <c r="U18">
+        <v>24</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>24</v>
+      </c>
+      <c r="X18">
+        <v>24</v>
+      </c>
+      <c r="Y18">
+        <v>2</v>
+      </c>
+      <c r="Z18">
+        <v>352</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <v>352</v>
+      </c>
+      <c r="AC18">
+        <v>352</v>
+      </c>
+      <c r="AD18">
+        <v>7</v>
+      </c>
+      <c r="AE18">
+        <v>93.04</v>
+      </c>
+      <c r="AF18">
+        <v>91.02</v>
+      </c>
+      <c r="AG18">
+        <v>392</v>
+      </c>
+      <c r="AH18">
+        <v>29</v>
+      </c>
+      <c r="AI18">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>[SP:FPTA-MR000494-SP1]</v>
+      </c>
+      <c r="B19" t="str">
+        <v>a7b71ac6c315fdd6b55e1c1676a3117c2cd00353</v>
+      </c>
+      <c r="C19" t="str">
+        <v>https://gerrit.ericsson.se/q/commit:a7b71ac6c315fdd6b55e1c1676a3117c2cd00353</v>
+      </c>
+      <c r="D19" t="str">
+        <v>gerrit</v>
+      </c>
+      <c r="E19" t="str">
+        <v>ehsxmng</v>
+      </c>
+      <c r="F19" t="str">
+        <v>Ming-Chen Hsu</v>
+      </c>
+      <c r="G19" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="H19" t="str">
+        <v>Unknown</v>
+      </c>
+      <c r="I19" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="J19" t="str">
+        <v>5g/src/rpcppg2</v>
+      </c>
+      <c r="K19" t="str">
+        <v>MSRBS</v>
+      </c>
+      <c r="L19" t="str">
+        <v>[SP:FPTA-MR000494-SP1] Removing nrCaSchedOptimForExtScellsEnable</v>
+      </c>
+      <c r="M19" t="str">
+        <v>2024-02-06</v>
+      </c>
+      <c r="N19" t="str">
+        <v>2024-02-06</v>
+      </c>
+      <c r="O19" t="str">
+        <v>source</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>180</v>
+      </c>
+      <c r="R19">
+        <v>-179</v>
+      </c>
+      <c r="S19">
+        <v>181</v>
+      </c>
+      <c r="T19">
+        <v>5</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>1</v>
+      </c>
+      <c r="AA19">
+        <v>180</v>
+      </c>
+      <c r="AB19">
+        <v>-179</v>
+      </c>
+      <c r="AC19">
+        <v>181</v>
+      </c>
+      <c r="AD19">
+        <v>5</v>
+      </c>
+      <c r="AE19">
+        <v>93.04</v>
+      </c>
+      <c r="AF19">
+        <v>95.89</v>
+      </c>
+      <c r="AG19">
+        <v>392</v>
+      </c>
+      <c r="AH19">
+        <v>0</v>
+      </c>
+      <c r="AI19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>[SP:11023-SP2]</v>
+      </c>
+      <c r="B20" t="str">
+        <v>bc68b6a23f66c359faa95e301698d9a198c918d0</v>
+      </c>
+      <c r="C20" t="str">
+        <v>https://gerrit.ericsson.se/q/commit:bc68b6a23f66c359faa95e301698d9a198c918d0</v>
+      </c>
+      <c r="D20" t="str">
+        <v>gerrit</v>
+      </c>
+      <c r="E20" t="str">
+        <v>ehsxmng</v>
+      </c>
+      <c r="F20" t="str">
+        <v>Ming-Chen Hsu</v>
+      </c>
+      <c r="G20" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="H20" t="str">
+        <v>Unknown</v>
+      </c>
+      <c r="I20" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="J20" t="str">
+        <v>lte/ebb</v>
+      </c>
+      <c r="K20" t="str">
+        <v>MSRBS</v>
+      </c>
+      <c r="L20" t="str">
+        <v>[SP:11023-SP2] Small delayTx for Response Handling</v>
+      </c>
+      <c r="M20" t="str">
+        <v>2024-03-14</v>
+      </c>
+      <c r="N20" t="str">
+        <v>2024-03-14</v>
+      </c>
+      <c r="O20" t="str">
+        <v>source test</v>
+      </c>
+      <c r="P20">
+        <v>124</v>
+      </c>
+      <c r="Q20">
+        <v>29</v>
+      </c>
+      <c r="R20">
+        <v>95</v>
+      </c>
+      <c r="S20">
+        <v>153</v>
+      </c>
+      <c r="T20">
+        <v>6</v>
+      </c>
+      <c r="U20">
+        <v>511</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>511</v>
+      </c>
+      <c r="X20">
+        <v>511</v>
+      </c>
+      <c r="Y20">
+        <v>1</v>
+      </c>
+      <c r="Z20">
+        <v>635</v>
+      </c>
+      <c r="AA20">
+        <v>29</v>
+      </c>
+      <c r="AB20">
+        <v>606</v>
+      </c>
+      <c r="AC20">
+        <v>664</v>
+      </c>
+      <c r="AD20">
+        <v>7</v>
+      </c>
+      <c r="AE20">
+        <v>97</v>
+      </c>
+      <c r="AF20">
+        <v>100</v>
+      </c>
+      <c r="AG20">
+        <v>429</v>
+      </c>
+      <c r="AH20">
+        <v>37</v>
+      </c>
+      <c r="AI20">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>[PC]</v>
+      </c>
+      <c r="B21" t="str">
+        <v>55e9065adf904372329f87ba3e2b25929529a8a1</v>
+      </c>
+      <c r="C21" t="str">
+        <v>https://gerrit.ericsson.se/q/commit:55e9065adf904372329f87ba3e2b25929529a8a1</v>
+      </c>
+      <c r="D21" t="str">
+        <v>gerrit</v>
+      </c>
+      <c r="E21" t="str">
+        <v>ehsxmng</v>
+      </c>
+      <c r="F21" t="str">
+        <v>Ming-Chen Hsu</v>
+      </c>
+      <c r="G21" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="H21" t="str">
+        <v>Unknown</v>
+      </c>
+      <c r="I21" t="str">
+        <v>unknown</v>
+      </c>
+      <c r="J21" t="str">
+        <v>5g/src/rpcppg2</v>
+      </c>
+      <c r="K21" t="str">
+        <v>MSRBS</v>
+      </c>
+      <c r="L21" t="str">
+        <v>[PC] MCT test for SrHandling</v>
+      </c>
+      <c r="M21" t="str">
+        <v>2024-05-27</v>
+      </c>
+      <c r="N21" t="str">
+        <v>2024-05-27</v>
+      </c>
+      <c r="O21" t="str">
+        <v>test</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>386</v>
+      </c>
+      <c r="V21">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>385</v>
+      </c>
+      <c r="X21">
+        <v>387</v>
+      </c>
+      <c r="Y21">
+        <v>1</v>
+      </c>
+      <c r="Z21">
+        <v>386</v>
+      </c>
+      <c r="AA21">
+        <v>1</v>
+      </c>
+      <c r="AB21">
+        <v>385</v>
+      </c>
+      <c r="AC21">
+        <v>387</v>
+      </c>
+      <c r="AD21">
+        <v>1</v>
+      </c>
+      <c r="AE21">
+        <v>100</v>
+      </c>
+      <c r="AF21">
+        <v>100</v>
+      </c>
+      <c r="AG21">
+        <v>503</v>
+      </c>
+      <c r="AH21">
+        <v>74</v>
+      </c>
+      <c r="AI21">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="AJ22">
+        <v>503</v>
+      </c>
+      <c r="AK22" t="str">
+        <v>2023-01-10</v>
+      </c>
+      <c r="AL22" t="str">
+        <v>2024-05-27</v>
+      </c>
+      <c r="AM22">
+        <v>3720</v>
+      </c>
+      <c r="AN22">
+        <v>12908</v>
+      </c>
+      <c r="AO22">
+        <v>16628</v>
+      </c>
+      <c r="AP22">
+        <v>23.95</v>
+      </c>
+      <c r="AQ22">
+        <v>177.14</v>
+      </c>
+      <c r="AR22">
+        <v>614.67</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AR5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AR22"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>